<commit_message>
add print client report
</commit_message>
<xml_diff>
--- a/Donot_Change/Stock.xlsx
+++ b/Donot_Change/Stock.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed-Tuf-PC\Documents\NetBeansProjects\new_mizan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed-Lap\Documents\NetBeansProjects\mizan_Java\Donot_Change\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2150547B-1548-458D-AB9A-755969FF8180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -45,7 +44,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -90,7 +89,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -99,6 +98,121 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -111,135 +225,10 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -248,46 +237,52 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -603,48 +598,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD9694F-ACC5-43EA-B067-9F4C9485653E}">
-  <dimension ref="A1:G29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E2"/>
+      <selection activeCell="E1" sqref="B1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="17" style="16" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
@@ -667,228 +662,147 @@
     </row>
     <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="8"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
       <c r="E7" s="6"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
-      <c r="B8" s="12"/>
+      <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
-      <c r="E8" s="6"/>
+      <c r="E8" s="7"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
-      <c r="B9" s="12"/>
+      <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="6"/>
+      <c r="E9" s="7"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
-      <c r="B10" s="12"/>
+      <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="6"/>
+      <c r="E10" s="7"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
-      <c r="B11" s="12"/>
+      <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="6"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
-      <c r="B12" s="12"/>
+      <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="6"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
-      <c r="B13" s="12"/>
+      <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="8"/>
+      <c r="E13" s="7"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
-      <c r="B14" s="11"/>
+      <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
-      <c r="E14" s="6"/>
+      <c r="E14" s="7"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
-      <c r="B15" s="12"/>
+      <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
-      <c r="E15" s="6"/>
+      <c r="E15" s="7"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="10"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
used static functions,highlight in stock table
</commit_message>
<xml_diff>
--- a/Donot_Change/Stock.xlsx
+++ b/Donot_Change/Stock.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed-Tuf-PC\Documents\NetBeansProjects\new_mizan\Donot_Change\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151E85C9-6138-4E37-BBAA-53958943824D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9326820-39B6-48B7-83A9-6E8C86221C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -290,7 +290,38 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -304,9 +335,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -344,7 +375,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -450,7 +481,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -592,7 +623,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -603,7 +634,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,6 +841,11 @@
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>
   </mergeCells>
+  <conditionalFormatting sqref="C5:C50 D5:D50 E5:E50">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$F5</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>